<commit_message>
up web bán hàng
</commit_message>
<xml_diff>
--- a/ExportExcel.xlsx
+++ b/ExportExcel.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="DSHH" sheetId="1" r:id="rId4"/>
+    <sheet name="DSLS" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -15,63 +15,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
-  <si>
-    <t>Mã Nhân Viên</t>
-  </si>
-  <si>
-    <t>Tên Nhân Viên</t>
-  </si>
-  <si>
-    <t>Giới Tính</t>
-  </si>
-  <si>
-    <t>Ngày Sinh</t>
-  </si>
-  <si>
-    <t>Điện Thoại</t>
-  </si>
-  <si>
-    <t>Địa Chỉ</t>
-  </si>
-  <si>
-    <t>Phòng Ban</t>
-  </si>
-  <si>
-    <t>CN-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Đinh Ngọc Ánh</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>2005-03-09</t>
-  </si>
-  <si>
-    <t>035765443</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t>Kế Toán</t>
-  </si>
-  <si>
-    <t>NV-01</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Quyen</t>
+  </si>
+  <si>
+    <t>Matkhau</t>
+  </si>
+  <si>
+    <t>Ngaytao</t>
+  </si>
+  <si>
+    <t>i@gmail.com</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>anhkk</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Khách hàng</t>
+  </si>
+  <si>
+    <t>mk</t>
+  </si>
+  <si>
+    <t>quynh181204@gmail.com</t>
   </si>
   <si>
     <t>quynh</t>
-  </si>
-  <si>
-    <t>2024-06-06</t>
-  </si>
-  <si>
-    <t>hanoi</t>
-  </si>
-  <si>
-    <t>Sale</t>
   </si>
 </sst>
 </file>
@@ -436,24 +418,21 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="9.283447" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,60 +445,50 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2">
-        <v>53</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
+        <v>993</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>